<commit_message>
finished consumption db import, linked to ei and ex
</commit_message>
<xml_diff>
--- a/consumption_model_ch/data/agribalyse_replaced_with_ecoinvent.xlsx
+++ b/consumption_model_ch/data/agribalyse_replaced_with_ecoinvent.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akim/PycharmProjects/consumption_model/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akim/PycharmProjects/consumption_model_ch/consumption_model_ch/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF2B147-7412-284F-B5AD-6F020100321E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6360F27-3B95-034F-B8F2-534761DB38BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1740" yWindow="-23540" windowWidth="32760" windowHeight="23380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="50">
   <si>
     <t>database</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>FR</t>
+  </si>
+  <si>
+    <t>egg</t>
+  </si>
+  <si>
+    <t>sea bass or sea bream</t>
+  </si>
+  <si>
+    <t>large trout</t>
+  </si>
+  <si>
+    <t>small trout</t>
   </si>
 </sst>
 </file>
@@ -544,7 +556,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -596,6 +608,9 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -667,6 +682,9 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
       <c r="C11" t="s">
         <v>45</v>
       </c>
@@ -721,6 +739,9 @@
       <c r="A15" t="s">
         <v>2</v>
       </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -792,7 +813,9 @@
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
       <c r="C22" t="s">
         <v>45</v>
       </c>
@@ -847,6 +870,9 @@
       <c r="A26" t="s">
         <v>2</v>
       </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -918,6 +944,9 @@
       <c r="A33" t="s">
         <v>11</v>
       </c>
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
       <c r="C33" t="s">
         <v>45</v>
       </c>
@@ -972,6 +1001,9 @@
       <c r="A37" t="s">
         <v>2</v>
       </c>
+      <c r="B37" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -1042,6 +1074,9 @@
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>12</v>
+      </c>
+      <c r="B44" t="s">
+        <v>49</v>
       </c>
       <c r="C44" t="s">
         <v>45</v>

</xml_diff>